<commit_message>
checking in patent code -- first take
</commit_message>
<xml_diff>
--- a/data/orgs/assignees_lookedup_types.xlsx
+++ b/data/orgs/assignees_lookedup_types.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34340" yWindow="2640" windowWidth="32560" windowHeight="20460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="5840" yWindow="2640" windowWidth="32560" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="assignees_lookedup_types" sheetId="1" r:id="rId1"/>
@@ -5830,11 +5830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E1789"/>
   <sheetViews>
-    <sheetView topLeftCell="A1785" zoomScale="143" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B1789"/>
+    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6340,7 +6339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -6527,7 +6526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
@@ -6824,7 +6823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>88</v>
       </c>
@@ -6835,7 +6834,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>89</v>
       </c>
@@ -7319,7 +7318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>133</v>
       </c>
@@ -7330,7 +7329,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>134</v>
       </c>
@@ -7341,7 +7340,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>135</v>
       </c>
@@ -7638,7 +7637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>162</v>
       </c>
@@ -7693,7 +7692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>167</v>
       </c>
@@ -7858,7 +7857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>182</v>
       </c>
@@ -7902,7 +7901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>186</v>
       </c>
@@ -8840,7 +8839,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="273" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>271</v>
       </c>
@@ -9118,7 +9117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="298" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>296</v>
       </c>
@@ -9495,7 +9494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="332" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>330</v>
       </c>
@@ -9902,7 +9901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="369" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>367</v>
       </c>
@@ -10081,7 +10080,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="385" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>383</v>
       </c>
@@ -11019,7 +11018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="470" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A470">
         <v>468</v>
       </c>
@@ -12537,7 +12536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="608" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="608" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A608">
         <v>606</v>
       </c>
@@ -12548,7 +12547,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="609" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="609" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A609">
         <v>607</v>
       </c>
@@ -14017,7 +14016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="742" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="742" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A742">
         <v>740</v>
       </c>
@@ -14050,7 +14049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="745" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="745" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A745">
         <v>743</v>
       </c>
@@ -14061,7 +14060,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="746" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="746" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A746">
         <v>744</v>
       </c>
@@ -14083,7 +14082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="748" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="748" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A748">
         <v>746</v>
       </c>
@@ -14094,7 +14093,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="749" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="749" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A749">
         <v>747</v>
       </c>
@@ -14116,7 +14115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="751" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="751" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A751">
         <v>749</v>
       </c>
@@ -14372,7 +14371,7 @@
         <v>1793</v>
       </c>
     </row>
-    <row r="774" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="774" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A774">
         <v>772</v>
       </c>
@@ -14430,7 +14429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="779" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="779" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A779">
         <v>777</v>
       </c>
@@ -14444,7 +14443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="780" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="780" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A780">
         <v>778</v>
       </c>
@@ -14458,7 +14457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="781" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="781" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A781">
         <v>779</v>
       </c>
@@ -14472,7 +14471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="782" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="782" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A782">
         <v>780</v>
       </c>
@@ -14486,7 +14485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="783" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="783" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A783">
         <v>781</v>
       </c>
@@ -14654,7 +14653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="798" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="798" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A798">
         <v>796</v>
       </c>
@@ -15468,7 +15467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="872" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="872" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A872">
         <v>870</v>
       </c>
@@ -15501,7 +15500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="875" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="875" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A875">
         <v>873</v>
       </c>
@@ -15611,7 +15610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="885" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="885" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A885">
         <v>883</v>
       </c>
@@ -15622,7 +15621,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="886" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="886" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A886">
         <v>884</v>
       </c>
@@ -15677,7 +15676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="891" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="891" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A891">
         <v>889</v>
       </c>
@@ -15732,7 +15731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="896" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="896" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A896">
         <v>894</v>
       </c>
@@ -15941,7 +15940,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="915" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="915" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A915">
         <v>913</v>
       </c>
@@ -16117,7 +16116,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="931" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="931" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A931">
         <v>929</v>
       </c>
@@ -16150,7 +16149,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="934" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="934" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A934">
         <v>932</v>
       </c>
@@ -16260,7 +16259,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="944" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="944" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A944">
         <v>942</v>
       </c>
@@ -16315,7 +16314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="949" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="949" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A949">
         <v>947</v>
       </c>
@@ -16348,7 +16347,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="952" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="952" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A952">
         <v>950</v>
       </c>
@@ -16403,7 +16402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="957" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="957" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A957">
         <v>955</v>
       </c>
@@ -16447,7 +16446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="961" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="961" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A961">
         <v>959</v>
       </c>
@@ -16469,7 +16468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="963" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="963" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A963">
         <v>961</v>
       </c>
@@ -16502,7 +16501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="966" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="966" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A966">
         <v>964</v>
       </c>
@@ -16590,7 +16589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="974" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="974" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A974">
         <v>972</v>
       </c>
@@ -16645,7 +16644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="979" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="979" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A979">
         <v>977</v>
       </c>
@@ -16656,7 +16655,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="980" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="980" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A980">
         <v>978</v>
       </c>
@@ -16689,7 +16688,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="983" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="983" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A983">
         <v>981</v>
       </c>
@@ -16722,7 +16721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="986" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="986" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A986">
         <v>984</v>
       </c>
@@ -16824,7 +16823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="995" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="995" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A995">
         <v>993</v>
       </c>
@@ -16835,7 +16834,7 @@
         <v>1794</v>
       </c>
     </row>
-    <row r="996" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="996" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A996">
         <v>994</v>
       </c>
@@ -16846,7 +16845,7 @@
         <v>1794</v>
       </c>
     </row>
-    <row r="997" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="997" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A997">
         <v>995</v>
       </c>
@@ -16890,7 +16889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1001" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1001" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1001">
         <v>999</v>
       </c>
@@ -16912,7 +16911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1003" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1003" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1003">
         <v>1001</v>
       </c>
@@ -16923,7 +16922,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1004" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1004" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1004">
         <v>1002</v>
       </c>
@@ -16967,7 +16966,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1008" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1008" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1008">
         <v>1006</v>
       </c>
@@ -16978,7 +16977,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1009" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1009" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1009">
         <v>1007</v>
       </c>
@@ -17000,7 +16999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1011" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1011" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1011">
         <v>1009</v>
       </c>
@@ -17011,7 +17010,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1012" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1012" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1012">
         <v>1010</v>
       </c>
@@ -17022,7 +17021,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1013" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1013" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1013">
         <v>1011</v>
       </c>
@@ -17058,7 +17057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1016" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1016" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1016">
         <v>1014</v>
       </c>
@@ -17135,7 +17134,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1023" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1023" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1023">
         <v>1021</v>
       </c>
@@ -17146,7 +17145,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1024" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1024" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1024">
         <v>1022</v>
       </c>
@@ -17168,7 +17167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1026" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1026" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1026">
         <v>1024</v>
       </c>
@@ -17215,7 +17214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1030" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1030" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1030">
         <v>1028</v>
       </c>
@@ -17391,7 +17390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1046" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1046" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1046">
         <v>1044</v>
       </c>
@@ -17446,7 +17445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1051" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1051" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1051">
         <v>1049</v>
       </c>
@@ -17578,7 +17577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1063" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1063" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1063">
         <v>1061</v>
       </c>
@@ -17600,7 +17599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1065" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1065" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1065">
         <v>1063</v>
       </c>
@@ -17611,7 +17610,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1066" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1066" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1066">
         <v>1064</v>
       </c>
@@ -17776,7 +17775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1081" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1081" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1081">
         <v>1079</v>
       </c>
@@ -17842,7 +17841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1087" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1087" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1087">
         <v>1085</v>
       </c>
@@ -17853,7 +17852,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1088" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1088" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1088">
         <v>1086</v>
       </c>
@@ -17864,7 +17863,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1089" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1089" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1089">
         <v>1087</v>
       </c>
@@ -17922,7 +17921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1094" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1094" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1094">
         <v>1092</v>
       </c>
@@ -18109,7 +18108,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1111" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1111">
         <v>1109</v>
       </c>
@@ -18186,7 +18185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1118" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1118">
         <v>1116</v>
       </c>
@@ -18219,7 +18218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1121" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1121">
         <v>1119</v>
       </c>
@@ -18230,7 +18229,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1122" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1122">
         <v>1120</v>
       </c>
@@ -18241,7 +18240,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1123" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1123">
         <v>1121</v>
       </c>
@@ -18516,7 +18515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1148" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1148">
         <v>1146</v>
       </c>
@@ -18527,7 +18526,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1149" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1149">
         <v>1147</v>
       </c>
@@ -18662,7 +18661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1161" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1161">
         <v>1159</v>
       </c>
@@ -18833,7 +18832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1176" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1176">
         <v>1174</v>
       </c>
@@ -18921,7 +18920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1184" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1184">
         <v>1182</v>
       </c>
@@ -19067,7 +19066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1197" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1197">
         <v>1195</v>
       </c>
@@ -19122,7 +19121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1202" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1202">
         <v>1200</v>
       </c>
@@ -19144,7 +19143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1204" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1204">
         <v>1202</v>
       </c>
@@ -19254,7 +19253,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1214" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1214">
         <v>1212</v>
       </c>
@@ -19265,7 +19264,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1215" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1215">
         <v>1213</v>
       </c>
@@ -19276,7 +19275,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1216" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1216">
         <v>1214</v>
       </c>
@@ -19287,7 +19286,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1217" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1217">
         <v>1215</v>
       </c>
@@ -19342,7 +19341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1222" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1222">
         <v>1220</v>
       </c>
@@ -19499,7 +19498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1236" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1236">
         <v>1234</v>
       </c>
@@ -19510,7 +19509,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1237" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1237">
         <v>1235</v>
       </c>
@@ -19590,7 +19589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1244" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1244">
         <v>1242</v>
       </c>
@@ -19684,7 +19683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1252" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1252">
         <v>1250</v>
       </c>
@@ -19728,7 +19727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1256" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1256">
         <v>1254</v>
       </c>
@@ -19770,7 +19769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1259" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1259">
         <v>1257</v>
       </c>
@@ -19847,7 +19846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1266" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1266">
         <v>1264</v>
       </c>
@@ -19858,7 +19857,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1267" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1267">
         <v>1265</v>
       </c>
@@ -19869,7 +19868,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1268" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1268">
         <v>1266</v>
       </c>
@@ -19880,7 +19879,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1269" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1269">
         <v>1267</v>
       </c>
@@ -19894,7 +19893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1270" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1270">
         <v>1268</v>
       </c>
@@ -19941,7 +19940,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1274" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1274">
         <v>1272</v>
       </c>
@@ -20035,7 +20034,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1282" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1282">
         <v>1280</v>
       </c>
@@ -20137,7 +20136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1291" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1291">
         <v>1289</v>
       </c>
@@ -20148,7 +20147,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1292" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1292">
         <v>1290</v>
       </c>
@@ -20162,7 +20161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1293" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1293">
         <v>1291</v>
       </c>
@@ -20311,7 +20310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1306" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1306">
         <v>1304</v>
       </c>
@@ -20325,7 +20324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1307" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1307">
         <v>1305</v>
       </c>
@@ -20339,7 +20338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1308" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1308">
         <v>1306</v>
       </c>
@@ -20361,7 +20360,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1310" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1310">
         <v>1308</v>
       </c>
@@ -20375,7 +20374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1311" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1311">
         <v>1309</v>
       </c>
@@ -20408,7 +20407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1314" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1314" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1314">
         <v>1312</v>
       </c>
@@ -20455,7 +20454,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1318" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1318" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1318">
         <v>1316</v>
       </c>
@@ -20500,7 +20499,7 @@
         <v>1798</v>
       </c>
     </row>
-    <row r="1321" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1321">
         <v>1319</v>
       </c>
@@ -20555,7 +20554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1326" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1326" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1326">
         <v>1324</v>
       </c>
@@ -20676,7 +20675,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1337" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1337" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1337">
         <v>1335</v>
       </c>
@@ -20690,7 +20689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1338" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1338" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1338">
         <v>1336</v>
       </c>
@@ -20704,7 +20703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1339" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1339" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1339">
         <v>1337</v>
       </c>
@@ -20715,7 +20714,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1340" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1340" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1340">
         <v>1338</v>
       </c>
@@ -20770,7 +20769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1345" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1345" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1345">
         <v>1343</v>
       </c>
@@ -20803,7 +20802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1348" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1348" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1348">
         <v>1346</v>
       </c>
@@ -20869,7 +20868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1354" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1354" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1354">
         <v>1352</v>
       </c>
@@ -20891,7 +20890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1356" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1356" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1356">
         <v>1354</v>
       </c>
@@ -20905,7 +20904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1357" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1357" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1357">
         <v>1355</v>
       </c>
@@ -20919,7 +20918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1358" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1358" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1358">
         <v>1356</v>
       </c>
@@ -20930,7 +20929,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1359" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1359" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1359">
         <v>1357</v>
       </c>
@@ -20944,7 +20943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1360" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1360" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1360">
         <v>1358</v>
       </c>
@@ -20955,7 +20954,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1361" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1361" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1361">
         <v>1359</v>
       </c>
@@ -21016,7 +21015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1366" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1366" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1366">
         <v>1364</v>
       </c>
@@ -21027,7 +21026,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1367" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1367" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1367">
         <v>1365</v>
       </c>
@@ -21115,7 +21114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1375" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1375" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1375">
         <v>1373</v>
       </c>
@@ -21225,7 +21224,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1385" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1385" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1385">
         <v>1383</v>
       </c>
@@ -21319,7 +21318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1393" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1393" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1393">
         <v>1391</v>
       </c>
@@ -21330,7 +21329,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1394" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1394" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1394">
         <v>1392</v>
       </c>
@@ -21484,7 +21483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1408" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1408" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1408">
         <v>1406</v>
       </c>
@@ -21638,7 +21637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1422" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1422">
         <v>1420</v>
       </c>
@@ -21649,7 +21648,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1423" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1423" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1423">
         <v>1421</v>
       </c>
@@ -21671,7 +21670,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1425" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1425" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1425">
         <v>1423</v>
       </c>
@@ -21825,7 +21824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1439" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1439" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1439">
         <v>1437</v>
       </c>
@@ -21880,7 +21879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1444" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1444" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1444">
         <v>1442</v>
       </c>
@@ -21891,7 +21890,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1445" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1445" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1445">
         <v>1443</v>
       </c>
@@ -21908,7 +21907,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="1446" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1446" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1446">
         <v>1444</v>
       </c>
@@ -21919,7 +21918,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1447" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1447" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1447">
         <v>1445</v>
       </c>
@@ -21944,7 +21943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1449" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1449" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1449">
         <v>1447</v>
       </c>
@@ -21975,7 +21974,7 @@
         <v>1799</v>
       </c>
     </row>
-    <row r="1451" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1451" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1451">
         <v>1449</v>
       </c>
@@ -22121,7 +22120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1464" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1464" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1464">
         <v>1462</v>
       </c>
@@ -22168,7 +22167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1468" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1468" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1468">
         <v>1466</v>
       </c>
@@ -22262,7 +22261,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1476" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1476" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1476">
         <v>1474</v>
       </c>
@@ -22387,7 +22386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1486" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1486" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1486">
         <v>1484</v>
       </c>
@@ -22415,7 +22414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1488" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1488" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1488">
         <v>1486</v>
       </c>
@@ -22597,7 +22596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1504" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1504" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1504">
         <v>1502</v>
       </c>
@@ -22743,7 +22742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1517" spans="1:4" s="4" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1517" spans="1:4" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1517" s="4">
         <v>1514.5</v>
       </c>
@@ -22878,7 +22877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1529" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1529" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1529">
         <v>1526</v>
       </c>
@@ -22903,7 +22902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1531" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1531" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1531">
         <v>1528</v>
       </c>
@@ -22928,7 +22927,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1533" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1533" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1533">
         <v>1530</v>
       </c>
@@ -22961,7 +22960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1536" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1536" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1536">
         <v>1533</v>
       </c>
@@ -22972,7 +22971,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1537" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1537" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1537">
         <v>1534</v>
       </c>
@@ -22983,7 +22982,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1538" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1538" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1538">
         <v>1535</v>
       </c>
@@ -23116,7 +23115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1549" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1549" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1549">
         <v>1546</v>
       </c>
@@ -23141,7 +23140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1551" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1551" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1551">
         <v>1548</v>
       </c>
@@ -23188,7 +23187,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1555" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1555" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1555">
         <v>1552</v>
       </c>
@@ -23235,7 +23234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1559" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1559" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1559">
         <v>1556</v>
       </c>
@@ -23279,7 +23278,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1563" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1563" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1563">
         <v>1560</v>
       </c>
@@ -23290,7 +23289,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1564" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1564" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1564">
         <v>1561</v>
       </c>
@@ -23469,7 +23468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1580" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1580" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1580">
         <v>1577</v>
       </c>
@@ -23483,7 +23482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1581" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1581" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1581">
         <v>1578</v>
       </c>
@@ -23494,7 +23493,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1582" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1582" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1582">
         <v>1579</v>
       </c>
@@ -23505,7 +23504,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1583" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1583" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1583">
         <v>1580</v>
       </c>
@@ -23516,7 +23515,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1584" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1584" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1584">
         <v>1581</v>
       </c>
@@ -23538,7 +23537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1586" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1586" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1586">
         <v>1583</v>
       </c>
@@ -23549,7 +23548,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1587" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1587" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1587">
         <v>1584</v>
       </c>
@@ -23560,7 +23559,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1588" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1588" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1588">
         <v>1585</v>
       </c>
@@ -23571,7 +23570,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1589" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1589" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1589">
         <v>1586</v>
       </c>
@@ -23582,7 +23581,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1590" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1590" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1590">
         <v>1587</v>
       </c>
@@ -23593,7 +23592,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1591" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1591" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1591">
         <v>1588</v>
       </c>
@@ -23604,7 +23603,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1592" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1592" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1592">
         <v>1589</v>
       </c>
@@ -23615,7 +23614,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1593" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1593" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1593">
         <v>1590</v>
       </c>
@@ -23637,7 +23636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1595" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1595" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1595">
         <v>1592</v>
       </c>
@@ -23648,7 +23647,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1596" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1596" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1596">
         <v>1593</v>
       </c>
@@ -23659,7 +23658,7 @@
         <v>1794</v>
       </c>
     </row>
-    <row r="1597" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1597" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1597">
         <v>1594</v>
       </c>
@@ -23673,7 +23672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1598" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1598" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1598">
         <v>1595</v>
       </c>
@@ -23687,7 +23686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1599" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1599" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1599">
         <v>1596</v>
       </c>
@@ -23701,7 +23700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1600" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1600" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1600">
         <v>1597</v>
       </c>
@@ -23723,7 +23722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1602" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1602" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1602">
         <v>1599</v>
       </c>
@@ -23745,7 +23744,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1604" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1604" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1604">
         <v>1601</v>
       </c>
@@ -23762,7 +23761,7 @@
         <v>1802</v>
       </c>
     </row>
-    <row r="1605" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1605" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1605">
         <v>1602</v>
       </c>
@@ -23784,7 +23783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1607" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1607" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1607">
         <v>1604</v>
       </c>
@@ -23795,7 +23794,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1608" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1608" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1608">
         <v>1605</v>
       </c>
@@ -23806,7 +23805,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1609" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1609" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1609">
         <v>1606</v>
       </c>
@@ -23828,7 +23827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1611" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1611" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1611">
         <v>1608</v>
       </c>
@@ -23859,7 +23858,7 @@
         <v>1803</v>
       </c>
     </row>
-    <row r="1613" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1613" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1613">
         <v>1610</v>
       </c>
@@ -23873,7 +23872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1614" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1614" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1614">
         <v>1611</v>
       </c>
@@ -23884,7 +23883,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1615" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1615" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1615">
         <v>1612</v>
       </c>
@@ -23895,7 +23894,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1616" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1616" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1616">
         <v>1613</v>
       </c>
@@ -23917,7 +23916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1618" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1618" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1618">
         <v>1615</v>
       </c>
@@ -23939,7 +23938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1620" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1620" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1620">
         <v>1617</v>
       </c>
@@ -23950,7 +23949,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1621" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1621" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1621">
         <v>1618</v>
       </c>
@@ -23961,7 +23960,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1622" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1622" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1622">
         <v>1619</v>
       </c>
@@ -23972,7 +23971,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1623" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1623" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1623">
         <v>1620</v>
       </c>
@@ -23983,7 +23982,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1624" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1624" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1624">
         <v>1621</v>
       </c>
@@ -23994,7 +23993,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1625" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1625" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1625">
         <v>1622</v>
       </c>
@@ -24005,7 +24004,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1626" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1626" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1626">
         <v>1623</v>
       </c>
@@ -24019,7 +24018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1627" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1627" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1627">
         <v>1624</v>
       </c>
@@ -24030,7 +24029,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1628" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1628" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1628">
         <v>1625</v>
       </c>
@@ -24041,7 +24040,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1629" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1629" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1629">
         <v>1626</v>
       </c>
@@ -24052,7 +24051,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1630" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1630" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1630">
         <v>1627</v>
       </c>
@@ -24063,7 +24062,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1631" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1631" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1631">
         <v>1628</v>
       </c>
@@ -24074,7 +24073,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1632" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1632" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1632">
         <v>1629</v>
       </c>
@@ -24085,7 +24084,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1633" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1633" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1633">
         <v>1630</v>
       </c>
@@ -24096,7 +24095,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1634" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1634" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1634">
         <v>1631</v>
       </c>
@@ -24107,7 +24106,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1635" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1635" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1635">
         <v>1632</v>
       </c>
@@ -24118,7 +24117,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1636" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1636" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1636">
         <v>1633</v>
       </c>
@@ -24129,7 +24128,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1637" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1637" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1637">
         <v>1634</v>
       </c>
@@ -24140,7 +24139,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1638" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1638" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1638">
         <v>1635</v>
       </c>
@@ -24151,7 +24150,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1639" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1639" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1639">
         <v>1636</v>
       </c>
@@ -24162,7 +24161,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1640" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1640" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1640">
         <v>1637</v>
       </c>
@@ -24173,7 +24172,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1641" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1641" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1641">
         <v>1638</v>
       </c>
@@ -24184,7 +24183,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1642" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1642" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1642">
         <v>1639</v>
       </c>
@@ -24195,7 +24194,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1643" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1643" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1643">
         <v>1640</v>
       </c>
@@ -24206,7 +24205,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1644" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1644" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1644">
         <v>1641</v>
       </c>
@@ -24217,7 +24216,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1645" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1645" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1645">
         <v>1642</v>
       </c>
@@ -24228,7 +24227,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1646" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1646" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1646">
         <v>1643</v>
       </c>
@@ -24239,7 +24238,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1647" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1647" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1647">
         <v>1644</v>
       </c>
@@ -24250,7 +24249,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1648" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1648" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1648">
         <v>1645</v>
       </c>
@@ -24261,7 +24260,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1649" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1649" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1649">
         <v>1646</v>
       </c>
@@ -24272,7 +24271,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1650" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1650" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1650">
         <v>1647</v>
       </c>
@@ -24283,7 +24282,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1651" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1651" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1651">
         <v>1648</v>
       </c>
@@ -24294,7 +24293,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1652" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1652" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1652">
         <v>1649</v>
       </c>
@@ -24305,7 +24304,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1653" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1653" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1653">
         <v>1650</v>
       </c>
@@ -24349,7 +24348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1657" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1657" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1657">
         <v>1654</v>
       </c>
@@ -24404,7 +24403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1662" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1662" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1662">
         <v>1659</v>
       </c>
@@ -24523,7 +24522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1672" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1672" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1672">
         <v>1669</v>
       </c>
@@ -24534,7 +24533,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1673" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1673" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1673">
         <v>1670</v>
       </c>
@@ -24545,7 +24544,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1674" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1674" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1674">
         <v>1671</v>
       </c>
@@ -24556,7 +24555,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1675" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1675" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1675">
         <v>1672</v>
       </c>
@@ -24639,7 +24638,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1682" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1682" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1682">
         <v>1679</v>
       </c>
@@ -24664,7 +24663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1684" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1684" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1684">
         <v>1681</v>
       </c>
@@ -24700,7 +24699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1687" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1687" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1687">
         <v>1684</v>
       </c>
@@ -24711,7 +24710,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1688" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1688" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1688">
         <v>1685</v>
       </c>
@@ -24843,7 +24842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1700" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1700" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1700">
         <v>1697</v>
       </c>
@@ -24854,7 +24853,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1701" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1701" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1701">
         <v>1698</v>
       </c>
@@ -24865,7 +24864,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1702" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1702" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1702">
         <v>1699</v>
       </c>
@@ -24876,7 +24875,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1703" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1703" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1703">
         <v>1700</v>
       </c>
@@ -24887,7 +24886,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1704" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1704" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1704">
         <v>1701</v>
       </c>
@@ -24898,7 +24897,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1705" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1705" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1705">
         <v>1702</v>
       </c>
@@ -24909,7 +24908,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1706" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1706" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1706">
         <v>1703</v>
       </c>
@@ -24920,7 +24919,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1707" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1707" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1707">
         <v>1704</v>
       </c>
@@ -24931,7 +24930,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1708" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1708" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1708">
         <v>1705</v>
       </c>
@@ -24942,7 +24941,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1709" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1709" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1709">
         <v>1706</v>
       </c>
@@ -24953,7 +24952,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1710" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1710" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1710">
         <v>1707</v>
       </c>
@@ -24964,7 +24963,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1711" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1711" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1711">
         <v>1708</v>
       </c>
@@ -24975,7 +24974,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1712" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1712" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1712">
         <v>1709</v>
       </c>
@@ -24986,7 +24985,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1713" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1713" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1713">
         <v>1710</v>
       </c>
@@ -24997,7 +24996,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1714" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1714" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1714">
         <v>1711</v>
       </c>
@@ -25008,7 +25007,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1715" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1715" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1715">
         <v>1712</v>
       </c>
@@ -25019,7 +25018,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1716" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1716" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1716">
         <v>1713</v>
       </c>
@@ -25030,7 +25029,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1717" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1717" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1717">
         <v>1714</v>
       </c>
@@ -25041,7 +25040,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1718" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1718" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1718">
         <v>1715</v>
       </c>
@@ -25052,7 +25051,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1719" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1719" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1719">
         <v>1716</v>
       </c>
@@ -25063,7 +25062,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1720" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1720" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1720">
         <v>1717</v>
       </c>
@@ -25074,7 +25073,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1721" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1721" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1721">
         <v>1718</v>
       </c>
@@ -25085,7 +25084,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1722" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1722" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1722">
         <v>1719</v>
       </c>
@@ -25096,7 +25095,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1723" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1723" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1723">
         <v>1720</v>
       </c>
@@ -25107,7 +25106,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1724" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1724" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1724">
         <v>1721</v>
       </c>
@@ -25118,7 +25117,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1725" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1725" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1725">
         <v>1722</v>
       </c>
@@ -25129,7 +25128,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1726" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1726" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1726">
         <v>1723</v>
       </c>
@@ -25140,7 +25139,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1727" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1727" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1727">
         <v>1724</v>
       </c>
@@ -25151,7 +25150,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1728" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1728" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1728">
         <v>1725</v>
       </c>
@@ -25162,7 +25161,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1729" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1729" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1729">
         <v>1726</v>
       </c>
@@ -25173,7 +25172,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1730" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1730" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1730">
         <v>1727</v>
       </c>
@@ -25184,7 +25183,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1731" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1731" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1731">
         <v>1728</v>
       </c>
@@ -25264,7 +25263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1738" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1738" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1738">
         <v>1735</v>
       </c>
@@ -25289,7 +25288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1740" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1740" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1740">
         <v>1737</v>
       </c>
@@ -25300,7 +25299,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1741" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1741" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1741">
         <v>1738</v>
       </c>
@@ -25405,7 +25404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1750" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1750" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1750">
         <v>1747</v>
       </c>
@@ -25416,7 +25415,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1751" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1751" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1751">
         <v>1748</v>
       </c>
@@ -25427,7 +25426,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1752" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1752" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1752">
         <v>1749</v>
       </c>
@@ -25438,7 +25437,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1753" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1753" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1753">
         <v>1750</v>
       </c>
@@ -25449,7 +25448,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1754" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1754" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1754">
         <v>1751</v>
       </c>
@@ -25493,7 +25492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1758" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1758" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1758">
         <v>1755</v>
       </c>
@@ -25529,7 +25528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1761" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1761" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1761">
         <v>1758</v>
       </c>
@@ -25540,7 +25539,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1762" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1762" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1762">
         <v>1759</v>
       </c>
@@ -25554,7 +25553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1763" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1763" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1763">
         <v>1760</v>
       </c>
@@ -25576,7 +25575,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1765" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1765" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1765">
         <v>1762</v>
       </c>
@@ -25587,7 +25586,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1766" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1766" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1766">
         <v>1763</v>
       </c>
@@ -25601,7 +25600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1767" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1767" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1767">
         <v>1764</v>
       </c>
@@ -25678,7 +25677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1774" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1774" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1774">
         <v>1771</v>
       </c>
@@ -25700,7 +25699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1776" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1776" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1776">
         <v>1773</v>
       </c>
@@ -25753,7 +25752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1780" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1780" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1780">
         <v>1777</v>
       </c>
@@ -25876,13 +25875,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1789">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Corporate"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D1789"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -25891,7 +25884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A1492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A401" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1492"/>
     </sheetView>
   </sheetViews>

</xml_diff>